<commit_message>
Done looking at Alt2
</commit_message>
<xml_diff>
--- a/Excel_Challenge_524 - Fill in Digits to make Perfect Square.xlsx
+++ b/Excel_Challenge_524 - Fill in Digits to make Perfect Square.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E1E78F-342F-4973-8BD3-88E066D84425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B57E52F-E188-4D9B-A8A5-4CE391268DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="20">
   <si>
     <t>Numbers</t>
   </si>
@@ -121,7 +121,10 @@
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7231147906508980224/</t>
   </si>
   <si>
-    <t>Same basic method as Alt1, but done correctly for work with 3 X numbers.</t>
+    <t>Same basic method as Alt1, but done correctly for work with 4 X numbers.</t>
+  </si>
+  <si>
+    <t>This is probably the most understandable, repeatable solution</t>
   </si>
 </sst>
 </file>
@@ -1381,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59D1A21-9CB5-4ED4-A442-79683EC47421}">
   <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,6 +1480,11 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
I don't think some of the solutions worked. Only 1 looks right and scalable
</commit_message>
<xml_diff>
--- a/Excel_Challenge_524 - Fill in Digits to make Perfect Square.xlsx
+++ b/Excel_Challenge_524 - Fill in Digits to make Perfect Square.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B57E52F-E188-4D9B-A8A5-4CE391268DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824D87DB-B221-4709-987C-028BFCE8B38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B2C357-EAB4-4E33-AE67-3358849D415B}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59D1A21-9CB5-4ED4-A442-79683EC47421}">
   <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>